<commit_message>
made changes in basetest
</commit_message>
<xml_diff>
--- a/crmSelenium/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
+++ b/crmSelenium/src/main/java/com/crm/qa/testdata/FreeCrmTestData.xlsx
@@ -9,20 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16640" tabRatio="500" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="contacts" sheetId="1" r:id="rId1"/>
-    <sheet name="deals" sheetId="2" r:id="rId2"/>
-    <sheet name="tasks" sheetId="3" r:id="rId3"/>
+    <sheet name="contacts" sheetId="1" r:id="rId3"/>
+    <sheet name="deals" sheetId="2" r:id="rId4"/>
+    <sheet name="tasks" sheetId="3" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <definedNames/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -46,50 +44,56 @@
     <t>Mr.</t>
   </si>
   <si>
-    <t>Tom</t>
-  </si>
-  <si>
-    <t>Peter</t>
-  </si>
-  <si>
-    <t>Google</t>
-  </si>
-  <si>
-    <t>Dr.</t>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Selvan</t>
+  </si>
+  <si>
+    <t>Salesforce</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Chris</t>
   </si>
   <si>
     <t>David</t>
   </si>
   <si>
-    <t>Cris</t>
-  </si>
-  <si>
-    <t>Amazon</t>
+    <t>Walmart</t>
   </si>
   <si>
     <t>Mrs.</t>
   </si>
   <si>
-    <t>Mukta</t>
+    <t>Anita</t>
   </si>
   <si>
     <t>Sharma</t>
   </si>
   <si>
-    <t>Ebay</t>
+    <t>Apple</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -123,21 +127,118 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -405,16 +506,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.255" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,7 +529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -442,7 +543,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -456,7 +557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -476,24 +577,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.255" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.255" defaultRowHeight="16"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>